<commit_message>
add toast message and fix bug
</commit_message>
<xml_diff>
--- a/FE/assets/Danh sách nhân viên.xlsx
+++ b/FE/assets/Danh sách nhân viên.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\projectInMisa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\projectInMisa\employeeManagement\FE\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FCF9F2-68D3-4A6B-9C04-7BB62D532B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82217C7-EC7F-44AF-9117-AADBA3BAAA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{966878AD-D04C-4658-BF65-867E2046772D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Danh sách nhân viên" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -452,11 +452,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,81 +772,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0874A6DD-AF38-4C5E-81FA-C42C1A2282CE}">
-  <dimension ref="A1:T13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26F0F7C-91D8-45AD-B25A-649469C89893}">
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+    <row r="2" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -902,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -958,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1014,7 +1004,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1070,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1126,7 +1116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1182,7 +1172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1238,7 +1228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1294,7 +1284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1350,7 +1340,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1406,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1416,7 +1406,7 @@
       <c r="C13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E13" s="3">
@@ -1464,7 +1454,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:T2"/>
+    <mergeCell ref="A1:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{842EA780-1A28-4F7E-A665-B8485FEAE3F4}"/>

</xml_diff>